<commit_message>
Added certain missing elements
</commit_message>
<xml_diff>
--- a/Patient Arrival Rate Plot.xlsx
+++ b/Patient Arrival Rate Plot.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17426"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bao\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luke Lattig\Desktop\New folder (2)\Repositories\CS273FinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$2:$L$34</definedName>
+  </definedNames>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
   <si>
     <t>Doctors:</t>
   </si>
@@ -49,11 +52,14 @@
   <si>
     <t>Trial 3</t>
   </si>
+  <si>
+    <t>Average Percentage:</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -103,6 +109,1323 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.10465706761696388"/>
+          <c:y val="4.145077720207254E-2"/>
+          <c:w val="0.77429096737283876"/>
+          <c:h val="0.8086241551412291"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="sysDash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$3:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>59</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$K$3:$K$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>7.5274800000000006</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.6151766666666667</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.66723</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.7776033333333343</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.8549800000000003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.1086933333333331</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.5408600000000003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.3909766666666652</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>11.431466666666665</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20.193733333333331</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20.399733333333334</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>17.050033333333332</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-EDA0-4882-96E0-E4E9BCAFA149}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="459923888"/>
+        <c:axId val="459918312"/>
+      </c:scatterChart>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Average Percentage</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="sysDash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$3:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>59</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$L$3:$L$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>99.961166666666671</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>99.939466666666661</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>99.909199999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>99.9298</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>99.913066666666666</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>99.940433333333331</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>99.790999999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>99.881033333333335</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>99.885733333333334</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>99.905166666666673</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>98.466533333333345</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>96.57053333333333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-EDA0-4882-96E0-E4E9BCAFA149}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="463020920"/>
+        <c:axId val="463015672"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="459923888"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Patients</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t>/hour</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="459918312"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="459918312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Average Wait Time (minutes)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="459923888"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="463015672"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Percentage</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> of Patients Treated</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="463020920"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="463020920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="463015672"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup orientation="landscape"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>28574</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>552449</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6EA8C455-FF73-455B-911C-C687B092CF56}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -181,6 +1504,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -216,6 +1556,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -368,10 +1725,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I14"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -381,9 +1741,11 @@
     <col min="3" max="3" width="10.85546875" customWidth="1"/>
     <col min="4" max="4" width="10.140625" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
+    <col min="11" max="11" width="17.85546875" customWidth="1"/>
+    <col min="12" max="12" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -403,8 +1765,14 @@
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
+      <c r="K1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
         <v>5</v>
       </c>
@@ -424,7 +1792,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>5</v>
       </c>
@@ -452,8 +1820,16 @@
       <c r="I3">
         <v>100</v>
       </c>
+      <c r="K3">
+        <f>(D3 + E3 + F3) /COUNTA(D3:F3)</f>
+        <v>7.5274800000000006</v>
+      </c>
+      <c r="L3">
+        <f>(G3+H3+I3)/COUNTA(G3:I3)</f>
+        <v>99.961166666666671</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>10</v>
       </c>
@@ -481,8 +1857,16 @@
       <c r="I4">
         <v>99.939599999999999</v>
       </c>
+      <c r="K4">
+        <f t="shared" ref="K4:K14" si="0">(D4 + E4 + F4) /COUNTA(D4:F4)</f>
+        <v>7.6151766666666667</v>
+      </c>
+      <c r="L4">
+        <f t="shared" ref="L4:L14" si="1">(G4+H4+I4)/COUNTA(G4:I4)</f>
+        <v>99.939466666666661</v>
+      </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>15</v>
       </c>
@@ -510,8 +1894,16 @@
       <c r="I5">
         <v>99.881600000000006</v>
       </c>
+      <c r="K5">
+        <f t="shared" si="0"/>
+        <v>7.66723</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="1"/>
+        <v>99.909199999999998</v>
+      </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>20</v>
       </c>
@@ -539,8 +1931,16 @@
       <c r="I6">
         <v>99.907799999999995</v>
       </c>
+      <c r="K6">
+        <f t="shared" si="0"/>
+        <v>7.7776033333333343</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="1"/>
+        <v>99.9298</v>
+      </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>25</v>
       </c>
@@ -568,8 +1968,16 @@
       <c r="I7">
         <v>99.951800000000006</v>
       </c>
+      <c r="K7">
+        <f t="shared" si="0"/>
+        <v>7.8549800000000003</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="1"/>
+        <v>99.913066666666666</v>
+      </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>30</v>
       </c>
@@ -579,8 +1987,34 @@
       <c r="C8">
         <v>5</v>
       </c>
+      <c r="D8">
+        <v>8.1323799999999995</v>
+      </c>
+      <c r="E8">
+        <v>8.0896100000000004</v>
+      </c>
+      <c r="F8">
+        <v>8.1040899999999993</v>
+      </c>
+      <c r="G8">
+        <v>99.939800000000005</v>
+      </c>
+      <c r="H8">
+        <v>99.920400000000001</v>
+      </c>
+      <c r="I8">
+        <v>99.961100000000002</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="0"/>
+        <v>8.1086933333333331</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="1"/>
+        <v>99.940433333333331</v>
+      </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>35</v>
       </c>
@@ -590,8 +2024,34 @@
       <c r="C9">
         <v>5</v>
       </c>
+      <c r="D9">
+        <v>8.5904000000000007</v>
+      </c>
+      <c r="E9">
+        <v>8.5332799999999995</v>
+      </c>
+      <c r="F9">
+        <v>8.4989000000000008</v>
+      </c>
+      <c r="G9">
+        <v>99.492999999999995</v>
+      </c>
+      <c r="H9">
+        <v>99.896900000000002</v>
+      </c>
+      <c r="I9">
+        <v>99.983099999999993</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="0"/>
+        <v>8.5408600000000003</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="1"/>
+        <v>99.790999999999997</v>
+      </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>40</v>
       </c>
@@ -601,8 +2061,34 @@
       <c r="C10">
         <v>5</v>
       </c>
+      <c r="D10">
+        <v>9.1963600000000003</v>
+      </c>
+      <c r="E10">
+        <v>9.7384699999999995</v>
+      </c>
+      <c r="F10">
+        <v>9.2380999999999993</v>
+      </c>
+      <c r="G10">
+        <v>99.865899999999996</v>
+      </c>
+      <c r="H10">
+        <v>99.865799999999993</v>
+      </c>
+      <c r="I10">
+        <v>99.9114</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="0"/>
+        <v>9.3909766666666652</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="1"/>
+        <v>99.881033333333335</v>
+      </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>45</v>
       </c>
@@ -612,8 +2098,34 @@
       <c r="C11">
         <v>5</v>
       </c>
+      <c r="D11">
+        <v>11.287100000000001</v>
+      </c>
+      <c r="E11">
+        <v>10.914300000000001</v>
+      </c>
+      <c r="F11">
+        <v>12.093</v>
+      </c>
+      <c r="G11">
+        <v>99.867999999999995</v>
+      </c>
+      <c r="H11">
+        <v>99.908100000000005</v>
+      </c>
+      <c r="I11">
+        <v>99.881100000000004</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="0"/>
+        <v>11.431466666666665</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="1"/>
+        <v>99.885733333333334</v>
+      </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>50</v>
       </c>
@@ -623,8 +2135,34 @@
       <c r="C12">
         <v>5</v>
       </c>
+      <c r="D12">
+        <v>18.3462</v>
+      </c>
+      <c r="E12">
+        <v>14.205299999999999</v>
+      </c>
+      <c r="F12">
+        <v>28.029699999999998</v>
+      </c>
+      <c r="G12">
+        <v>99.916899999999998</v>
+      </c>
+      <c r="H12">
+        <v>99.881699999999995</v>
+      </c>
+      <c r="I12">
+        <v>99.916899999999998</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="0"/>
+        <v>20.193733333333331</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="1"/>
+        <v>99.905166666666673</v>
+      </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>55</v>
       </c>
@@ -634,8 +2172,34 @@
       <c r="C13">
         <v>5</v>
       </c>
+      <c r="D13">
+        <v>22.828499999999998</v>
+      </c>
+      <c r="E13">
+        <v>21.955300000000001</v>
+      </c>
+      <c r="F13">
+        <v>16.415400000000002</v>
+      </c>
+      <c r="G13">
+        <v>98.420100000000005</v>
+      </c>
+      <c r="H13">
+        <v>98.259600000000006</v>
+      </c>
+      <c r="I13">
+        <v>98.719899999999996</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="0"/>
+        <v>20.399733333333334</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="1"/>
+        <v>98.466533333333345</v>
+      </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>59</v>
       </c>
@@ -644,6 +2208,32 @@
       </c>
       <c r="C14">
         <v>5</v>
+      </c>
+      <c r="D14">
+        <v>18.062899999999999</v>
+      </c>
+      <c r="E14">
+        <v>15.196400000000001</v>
+      </c>
+      <c r="F14">
+        <v>17.890799999999999</v>
+      </c>
+      <c r="G14">
+        <v>97.131299999999996</v>
+      </c>
+      <c r="H14">
+        <v>96.215900000000005</v>
+      </c>
+      <c r="I14">
+        <v>96.364400000000003</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="0"/>
+        <v>17.050033333333332</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="1"/>
+        <v>96.57053333333333</v>
       </c>
     </row>
   </sheetData>
@@ -652,5 +2242,7 @@
     <mergeCell ref="G1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="86" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>